<commit_message>
translation demo 66 + layout
</commit_message>
<xml_diff>
--- a/book/demos/Overview_demos.xlsx
+++ b/book/demos/Overview_demos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suzan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ella\Documents\TU\Git\Showing-Physics\book\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8248FA62-BD24-47FC-BCE6-2174B17AD22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C37C3BE-83B7-40D3-B498-0DDE5EBC8E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="180">
   <si>
     <t>Demo name</t>
   </si>
@@ -697,9 +697,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -737,7 +737,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -843,7 +843,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -985,7 +985,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,9 +995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2687,6 +2687,9 @@
         <v>76</v>
       </c>
       <c r="G81" s="2"/>
+      <c r="I81" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82">

</xml_diff>

<commit_message>
translation and markdown demo 63-66
</commit_message>
<xml_diff>
--- a/book/demos/Overview_demos.xlsx
+++ b/book/demos/Overview_demos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ella\Documents\TU\Git\Showing-Physics\book\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C37C3BE-83B7-40D3-B498-0DDE5EBC8E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38BA71E-B03E-4A98-8827-CE0C8D9B26A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="181">
   <si>
     <t>Demo name</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>Rich boiling phenomena</t>
+  </si>
+  <si>
+    <t>check age group</t>
   </si>
 </sst>
 </file>
@@ -995,9 +998,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2390,7 +2393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>50</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>51</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>52</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>53</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>54</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>55</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>56</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>57</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>58</v>
       </c>
@@ -2547,7 +2550,7 @@
       </c>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74">
         <v>59</v>
       </c>
@@ -2565,7 +2568,7 @@
       </c>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>60</v>
       </c>
@@ -2583,7 +2586,7 @@
       </c>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>61</v>
       </c>
@@ -2601,7 +2604,7 @@
       </c>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>62</v>
       </c>
@@ -2619,7 +2622,7 @@
       </c>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>63</v>
       </c>
@@ -2633,8 +2636,11 @@
         <v>79</v>
       </c>
       <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>64</v>
       </c>
@@ -2651,8 +2657,14 @@
         <v>78</v>
       </c>
       <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H79" t="s">
+        <v>180</v>
+      </c>
+      <c r="I79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>65</v>
       </c>
@@ -2669,6 +2681,9 @@
         <v>77</v>
       </c>
       <c r="G80" s="2"/>
+      <c r="I80" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81">
@@ -3386,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:F48"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
demo 81 added it in ipynb, translated and put into md: 58-60
</commit_message>
<xml_diff>
--- a/book/demos/Overview_demos.xlsx
+++ b/book/demos/Overview_demos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ella\Documents\TU\Git\Showing-Physics\book\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38BA71E-B03E-4A98-8827-CE0C8D9B26A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3396C58-C4B4-4D9C-9E62-D0949CD22BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="183">
   <si>
     <t>Demo name</t>
   </si>
@@ -569,6 +569,12 @@
   </si>
   <si>
     <t>check age group</t>
+  </si>
+  <si>
+    <t>no tekst yet</t>
+  </si>
+  <si>
+    <t>No tekst yet: or actually under demo 60</t>
   </si>
 </sst>
 </file>
@@ -998,9 +1004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
+      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2549,6 +2555,9 @@
         <v>73</v>
       </c>
       <c r="G73" s="2"/>
+      <c r="I73" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74">
@@ -2567,6 +2576,9 @@
         <v>72</v>
       </c>
       <c r="G74" s="2"/>
+      <c r="I74" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75">
@@ -2585,6 +2597,9 @@
         <v>71</v>
       </c>
       <c r="G75" s="2"/>
+      <c r="I75" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76">
@@ -2603,6 +2618,9 @@
         <v>70</v>
       </c>
       <c r="G76" s="2"/>
+      <c r="H76" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77">
@@ -2621,6 +2639,9 @@
         <v>119</v>
       </c>
       <c r="G77" s="6"/>
+      <c r="H77" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78">
@@ -3401,7 +3422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
translated and layout demo 55,56,61,62,67
</commit_message>
<xml_diff>
--- a/book/demos/Overview_demos.xlsx
+++ b/book/demos/Overview_demos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\book\demos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ella\Documents\TU\Git\Showing-Physics\book\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A378DA0-AA08-47EB-9C6B-FE100E65BB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0076F89-F8EB-4E2A-A579-FF5BD6E544BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1152" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="181">
   <si>
     <t>Demo name</t>
   </si>
@@ -547,9 +547,6 @@
     <t>nog een extra foto van binnenkant opstelling nodig</t>
   </si>
   <si>
-    <t>mis alle tekst</t>
-  </si>
-  <si>
     <t xml:space="preserve">tekst staat nog in ipynb </t>
   </si>
   <si>
@@ -571,10 +568,7 @@
     <t>check age group</t>
   </si>
   <si>
-    <t>no tekst yet</t>
-  </si>
-  <si>
-    <t>No tekst yet: or actually under demo 60</t>
+    <t>needs tekst</t>
   </si>
 </sst>
 </file>
@@ -1004,27 +998,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="7" width="81.28515625" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="7" width="81.33203125" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>134</v>
       </c>
@@ -1060,7 +1054,7 @@
       </c>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1077,7 +1071,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1094,7 +1088,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1111,7 +1105,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1129,7 +1123,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1147,7 +1141,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1165,7 +1159,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1185,7 +1179,7 @@
       </c>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1205,7 +1199,7 @@
       </c>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1225,7 +1219,7 @@
       </c>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1245,7 +1239,7 @@
       </c>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1263,7 +1257,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1276,7 +1270,7 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1289,7 +1283,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1302,7 +1296,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>1</v>
       </c>
@@ -1327,7 +1321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>2</v>
       </c>
@@ -1354,7 +1348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>3</v>
       </c>
@@ -1384,7 +1378,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>4</v>
       </c>
@@ -1407,7 +1401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>5</v>
       </c>
@@ -1432,7 +1426,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>6</v>
       </c>
@@ -1457,7 +1451,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>7</v>
       </c>
@@ -1482,7 +1476,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>8</v>
       </c>
@@ -1505,7 +1499,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>9</v>
       </c>
@@ -1528,7 +1522,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>10</v>
       </c>
@@ -1554,7 +1548,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>11</v>
       </c>
@@ -1580,7 +1574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>12</v>
       </c>
@@ -1606,7 +1600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>13</v>
       </c>
@@ -1629,7 +1623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>14</v>
       </c>
@@ -1658,7 +1652,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>15</v>
       </c>
@@ -1681,7 +1675,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>16</v>
       </c>
@@ -1704,7 +1698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>17</v>
       </c>
@@ -1727,7 +1721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>18</v>
       </c>
@@ -1753,7 +1747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>19</v>
       </c>
@@ -1777,7 +1771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>20</v>
       </c>
@@ -1804,7 +1798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>21</v>
       </c>
@@ -1828,7 +1822,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>22</v>
       </c>
@@ -1852,7 +1846,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>23</v>
       </c>
@@ -1876,7 +1870,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>24</v>
       </c>
@@ -1900,7 +1894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>25</v>
       </c>
@@ -1924,7 +1918,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>26</v>
       </c>
@@ -1944,7 +1938,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>27</v>
       </c>
@@ -1964,7 +1958,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>28</v>
       </c>
@@ -1984,7 +1978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>29</v>
       </c>
@@ -2004,7 +1998,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>30</v>
       </c>
@@ -2024,7 +2018,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>31</v>
       </c>
@@ -2044,7 +2038,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>32</v>
       </c>
@@ -2058,7 +2052,7 @@
         <v>37</v>
       </c>
       <c r="F47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H47" t="s">
         <v>139</v>
@@ -2067,7 +2061,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>33</v>
       </c>
@@ -2081,13 +2075,13 @@
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>34</v>
       </c>
@@ -2101,7 +2095,7 @@
         <v>57</v>
       </c>
       <c r="F49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H49" t="s">
         <v>141</v>
@@ -2110,7 +2104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>35</v>
       </c>
@@ -2124,13 +2118,13 @@
         <v>59</v>
       </c>
       <c r="F50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I50" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>36</v>
       </c>
@@ -2144,13 +2138,13 @@
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>37</v>
       </c>
@@ -2170,7 +2164,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>38</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>39</v>
       </c>
@@ -2210,7 +2204,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>40</v>
       </c>
@@ -2230,7 +2224,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>41</v>
       </c>
@@ -2250,7 +2244,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>42</v>
       </c>
@@ -2270,7 +2264,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>43</v>
       </c>
@@ -2290,7 +2284,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>44</v>
       </c>
@@ -2310,7 +2304,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>45</v>
       </c>
@@ -2327,7 +2321,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>46</v>
       </c>
@@ -2344,7 +2338,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>47</v>
       </c>
@@ -2362,7 +2356,7 @@
       </c>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>48</v>
       </c>
@@ -2382,7 +2376,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>49</v>
       </c>
@@ -2399,7 +2393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>50</v>
       </c>
@@ -2416,7 +2410,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>51</v>
       </c>
@@ -2436,7 +2430,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>52</v>
       </c>
@@ -2453,7 +2447,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>53</v>
       </c>
@@ -2470,7 +2464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>54</v>
       </c>
@@ -2487,7 +2481,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>55</v>
       </c>
@@ -2503,8 +2497,11 @@
       <c r="F70" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>56</v>
       </c>
@@ -2520,8 +2517,11 @@
       <c r="F71" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>57</v>
       </c>
@@ -2537,8 +2537,11 @@
       <c r="F72" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>58</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74">
         <v>59</v>
       </c>
@@ -2580,7 +2583,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>60</v>
       </c>
@@ -2597,14 +2600,11 @@
         <v>70</v>
       </c>
       <c r="G75" s="2"/>
-      <c r="H75" t="s">
-        <v>182</v>
-      </c>
       <c r="I75" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>61</v>
       </c>
@@ -2621,8 +2621,11 @@
         <v>71</v>
       </c>
       <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>62</v>
       </c>
@@ -2639,11 +2642,11 @@
         <v>119</v>
       </c>
       <c r="G77" s="6"/>
-      <c r="H77" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>63</v>
       </c>
@@ -2661,7 +2664,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>64</v>
       </c>
@@ -2679,13 +2682,13 @@
       </c>
       <c r="G79" s="2"/>
       <c r="H79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I79" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>65</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>66</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>67</v>
       </c>
@@ -2743,11 +2746,12 @@
       <c r="F82" t="s">
         <v>118</v>
       </c>
-      <c r="H82" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H82" s="6"/>
+      <c r="I82" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>68</v>
       </c>
@@ -2768,7 +2772,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>69</v>
       </c>
@@ -2785,7 +2789,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>70</v>
       </c>
@@ -2805,7 +2809,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>71</v>
       </c>
@@ -2825,7 +2829,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>72</v>
       </c>
@@ -2848,7 +2852,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>73</v>
       </c>
@@ -2865,10 +2869,10 @@
         <v>67</v>
       </c>
       <c r="H88" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B89">
         <v>74</v>
       </c>
@@ -2891,7 +2895,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B90">
         <v>75</v>
       </c>
@@ -2914,7 +2918,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B91">
         <v>76</v>
       </c>
@@ -2934,7 +2938,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B92">
         <v>77</v>
       </c>
@@ -2954,7 +2958,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B93">
         <v>78</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B94">
         <v>79</v>
       </c>
@@ -2994,7 +2998,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B95" s="1">
         <v>80</v>
       </c>
@@ -3018,7 +3022,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>81</v>
       </c>
@@ -3038,7 +3042,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B97" s="1">
         <v>82</v>
       </c>
@@ -3062,7 +3066,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B98">
         <v>83</v>
       </c>
@@ -3082,7 +3086,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B99">
         <v>84</v>
       </c>
@@ -3105,7 +3109,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B100">
         <v>85</v>
       </c>
@@ -3128,7 +3132,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B101">
         <v>86</v>
       </c>
@@ -3151,7 +3155,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B102">
         <v>87</v>
       </c>
@@ -3174,7 +3178,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>88</v>
       </c>
@@ -3194,7 +3198,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B104">
         <v>89</v>
       </c>
@@ -3217,7 +3221,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B105">
         <v>90</v>
       </c>
@@ -3234,7 +3238,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>91</v>
       </c>
@@ -3251,7 +3255,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>92</v>
       </c>
@@ -3268,7 +3272,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B108">
         <v>93</v>
       </c>
@@ -3285,7 +3289,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>94</v>
       </c>
@@ -3302,7 +3306,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B110">
         <v>95</v>
       </c>
@@ -3322,7 +3326,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>96</v>
       </c>
@@ -3345,7 +3349,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B112">
         <v>97</v>
       </c>
@@ -3362,7 +3366,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B113">
         <v>98</v>
       </c>
@@ -3385,7 +3389,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B114">
         <v>99</v>
       </c>
@@ -3402,13 +3406,13 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F118" s="6" t="s">
         <v>116</v>
       </c>
       <c r="G118" s="6"/>
     </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
     </row>
@@ -3426,21 +3430,21 @@
       <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="81.28515625" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="81.33203125" customWidth="1"/>
+    <col min="7" max="7" width="41.33203125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>134</v>
       </c>
@@ -3473,7 +3477,7 @@
       </c>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3490,7 +3494,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3507,7 +3511,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3524,7 +3528,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3541,7 +3545,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3558,7 +3562,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3575,7 +3579,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3594,7 +3598,7 @@
       </c>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3613,7 +3617,7 @@
       </c>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3632,7 +3636,7 @@
       </c>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3651,7 +3655,7 @@
       </c>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3668,7 +3672,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3685,7 +3689,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>1</v>
       </c>
@@ -3707,7 +3711,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>6</v>
       </c>
@@ -3729,7 +3733,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>8</v>
       </c>
@@ -3750,7 +3754,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>70</v>
       </c>
@@ -3772,7 +3776,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>71</v>
       </c>
@@ -3794,7 +3798,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>72</v>
       </c>
@@ -3816,7 +3820,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>91</v>
       </c>
@@ -3838,7 +3842,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -3850,7 +3854,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -3862,7 +3866,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>13</v>
       </c>
@@ -3879,7 +3883,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>9</v>
       </c>
@@ -3901,7 +3905,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>10</v>
       </c>
@@ -3923,7 +3927,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>39</v>
       </c>
@@ -3945,7 +3949,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>41</v>
       </c>
@@ -3967,7 +3971,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>73</v>
       </c>
@@ -3989,7 +3993,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>92</v>
       </c>
@@ -4011,7 +4015,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -4023,7 +4027,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -4035,7 +4039,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -4047,7 +4051,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>14</v>
       </c>
@@ -4064,7 +4068,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>3</v>
       </c>
@@ -4086,7 +4090,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>20</v>
       </c>
@@ -4108,7 +4112,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>21</v>
       </c>
@@ -4130,7 +4134,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>22</v>
       </c>
@@ -4152,7 +4156,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>23</v>
       </c>
@@ -4174,7 +4178,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>24</v>
       </c>
@@ -4196,7 +4200,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>33</v>
       </c>
@@ -4218,7 +4222,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>74</v>
       </c>
@@ -4240,7 +4244,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>77</v>
       </c>
@@ -4262,7 +4266,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>79</v>
       </c>
@@ -4284,7 +4288,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>80</v>
       </c>
@@ -4306,7 +4310,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>81</v>
       </c>
@@ -4328,7 +4332,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>83</v>
       </c>
@@ -4350,7 +4354,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>87</v>
       </c>
@@ -4372,7 +4376,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>89</v>
       </c>
@@ -4394,7 +4398,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -4406,7 +4410,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -4418,7 +4422,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -4430,7 +4434,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
@@ -4442,7 +4446,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
@@ -4454,7 +4458,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
@@ -4466,7 +4470,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
@@ -4478,7 +4482,7 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="56" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
@@ -4490,7 +4494,7 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
     </row>
-    <row r="57" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
@@ -4502,7 +4506,7 @@
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
     </row>
-    <row r="58" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
@@ -4514,7 +4518,7 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
@@ -4526,7 +4530,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
@@ -4538,7 +4542,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
@@ -4550,7 +4554,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -4562,7 +4566,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>15</v>
       </c>
@@ -4579,7 +4583,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -4591,7 +4595,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -4603,7 +4607,7 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -4615,7 +4619,7 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>16</v>
       </c>
@@ -4632,7 +4636,7 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -4644,7 +4648,7 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -4656,7 +4660,7 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -4668,7 +4672,7 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -4680,7 +4684,7 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -4692,7 +4696,7 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>17</v>
       </c>
@@ -4709,7 +4713,7 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -4721,7 +4725,7 @@
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
     </row>
-    <row r="75" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -4733,7 +4737,7 @@
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
     </row>
-    <row r="76" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -4745,7 +4749,7 @@
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
     </row>
-    <row r="77" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -4757,7 +4761,7 @@
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
     </row>
-    <row r="78" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -4769,7 +4773,7 @@
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
     </row>
-    <row r="79" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>18</v>
       </c>
@@ -4786,7 +4790,7 @@
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
     </row>
-    <row r="80" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -4798,7 +4802,7 @@
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
     </row>
-    <row r="81" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -4810,7 +4814,7 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
     </row>
-    <row r="82" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -4822,7 +4826,7 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
     </row>
-    <row r="83" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -4834,7 +4838,7 @@
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -4846,7 +4850,7 @@
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
     </row>
-    <row r="85" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>19</v>
       </c>
@@ -4863,7 +4867,7 @@
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
     </row>
-    <row r="86" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -4875,7 +4879,7 @@
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -4887,7 +4891,7 @@
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
     </row>
-    <row r="88" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -4899,7 +4903,7 @@
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
     </row>
-    <row r="89" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -4911,7 +4915,7 @@
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
     </row>
-    <row r="90" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -4923,7 +4927,7 @@
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
     </row>
-    <row r="91" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -4935,7 +4939,7 @@
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
     </row>
-    <row r="92" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -4947,7 +4951,7 @@
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
     </row>
-    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G93" s="3"/>
       <c r="H93" s="3" t="s">
         <v>31</v>
@@ -4956,7 +4960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="3">
         <v>2</v>
       </c>
@@ -4982,7 +4986,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G95" s="8" t="s">
         <v>10</v>
       </c>
@@ -4996,7 +5000,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>4</v>
       </c>
@@ -5019,7 +5023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>5</v>
       </c>
@@ -5043,7 +5047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B98">
         <v>7</v>
       </c>
@@ -5067,7 +5071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G99" s="2"/>
       <c r="H99" t="s">
         <v>31</v>
@@ -5076,7 +5080,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H100" t="s">
         <v>31</v>
       </c>
@@ -5084,7 +5088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H101" t="s">
         <v>31</v>
       </c>
@@ -5092,7 +5096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G102" t="s">
         <v>80</v>
       </c>
@@ -5103,7 +5107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>11</v>
       </c>
@@ -5129,7 +5133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B104">
         <v>12</v>
       </c>
@@ -5155,7 +5159,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B105">
         <v>13</v>
       </c>
@@ -5178,7 +5182,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>14</v>
       </c>
@@ -5207,7 +5211,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>15</v>
       </c>
@@ -5230,7 +5234,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B108">
         <v>16</v>
       </c>
@@ -5256,7 +5260,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>17</v>
       </c>
@@ -5279,7 +5283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B110">
         <v>18</v>
       </c>
@@ -5305,7 +5309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>19</v>
       </c>
@@ -5331,7 +5335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G112" t="s">
         <v>35</v>
       </c>
@@ -5342,7 +5346,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G113" s="1" t="s">
         <v>34</v>
       </c>
@@ -5353,7 +5357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G114" t="s">
         <v>34</v>
       </c>
@@ -5364,7 +5368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G115" s="1" t="s">
         <v>34</v>
       </c>
@@ -5375,7 +5379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G116" s="1" t="s">
         <v>34</v>
       </c>
@@ -5386,7 +5390,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B117">
         <v>25</v>
       </c>
@@ -5412,7 +5416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B118">
         <v>26</v>
       </c>
@@ -5432,7 +5436,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B119">
         <v>27</v>
       </c>
@@ -5452,7 +5456,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B120">
         <v>28</v>
       </c>
@@ -5472,7 +5476,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>29</v>
       </c>
@@ -5492,7 +5496,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>30</v>
       </c>
@@ -5512,7 +5516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B123">
         <v>31</v>
       </c>
@@ -5532,7 +5536,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>32</v>
       </c>
@@ -5555,12 +5559,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H125" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126">
         <v>34</v>
       </c>
@@ -5583,7 +5587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>35</v>
       </c>
@@ -5603,7 +5607,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>36</v>
       </c>
@@ -5623,7 +5627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B129">
         <v>37</v>
       </c>
@@ -5643,7 +5647,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>38</v>
       </c>
@@ -5663,12 +5667,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G131" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>40</v>
       </c>
@@ -5688,12 +5692,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G133" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>42</v>
       </c>
@@ -5713,7 +5717,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B135">
         <v>43</v>
       </c>
@@ -5733,7 +5737,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B136">
         <v>44</v>
       </c>
@@ -5753,7 +5757,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B137">
         <v>45</v>
       </c>
@@ -5770,7 +5774,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B138">
         <v>46</v>
       </c>
@@ -5787,7 +5791,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B139">
         <v>47</v>
       </c>
@@ -5804,7 +5808,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B140">
         <v>48</v>
       </c>
@@ -5824,7 +5828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B141">
         <v>49</v>
       </c>
@@ -5841,7 +5845,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B142">
         <v>50</v>
       </c>
@@ -5858,7 +5862,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B143">
         <v>51</v>
       </c>
@@ -5878,7 +5882,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B144">
         <v>52</v>
       </c>
@@ -5895,7 +5899,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B145">
         <v>53</v>
       </c>
@@ -5912,7 +5916,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B146">
         <v>54</v>
       </c>
@@ -5929,7 +5933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B147">
         <v>55</v>
       </c>
@@ -5946,7 +5950,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B148">
         <v>56</v>
       </c>
@@ -5963,7 +5967,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B149">
         <v>57</v>
       </c>
@@ -5980,7 +5984,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B150">
         <v>58</v>
       </c>
@@ -5997,7 +6001,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B151">
         <v>59</v>
       </c>
@@ -6014,7 +6018,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B152">
         <v>60</v>
       </c>
@@ -6031,7 +6035,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B153">
         <v>61</v>
       </c>
@@ -6048,7 +6052,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B154">
         <v>62</v>
       </c>
@@ -6065,7 +6069,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B155">
         <v>63</v>
       </c>
@@ -6079,7 +6083,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B156">
         <v>64</v>
       </c>
@@ -6096,7 +6100,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B157">
         <v>65</v>
       </c>
@@ -6113,7 +6117,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B158">
         <v>66</v>
       </c>
@@ -6130,7 +6134,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B159">
         <v>67</v>
       </c>
@@ -6148,7 +6152,7 @@
       </c>
       <c r="G159" s="6"/>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B160">
         <v>68</v>
       </c>
@@ -6165,7 +6169,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B161">
         <v>69</v>
       </c>
@@ -6179,7 +6183,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B167">
         <v>75</v>
       </c>
@@ -6196,7 +6200,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B168">
         <v>76</v>
       </c>
@@ -6213,7 +6217,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B170">
         <v>78</v>
       </c>
@@ -6230,7 +6234,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B174">
         <v>82</v>
       </c>
@@ -6247,7 +6251,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B176">
         <v>84</v>
       </c>
@@ -6264,7 +6268,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="177" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B177">
         <v>85</v>
       </c>
@@ -6281,7 +6285,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="178" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B178">
         <v>86</v>
       </c>
@@ -6298,7 +6302,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="180" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B180">
         <v>88</v>
       </c>
@@ -6315,7 +6319,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B182">
         <v>90</v>
       </c>
@@ -6332,7 +6336,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="185" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B185">
         <v>93</v>
       </c>
@@ -6349,7 +6353,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="186" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B186">
         <v>94</v>
       </c>
@@ -6366,7 +6370,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="187" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B187">
         <v>95</v>
       </c>
@@ -6386,7 +6390,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="188" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B188">
         <v>96</v>
       </c>
@@ -6409,7 +6413,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="189" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B189">
         <v>97</v>
       </c>
@@ -6426,7 +6430,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="190" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B190">
         <v>98</v>
       </c>
@@ -6449,7 +6453,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="191" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B191">
         <v>99</v>
       </c>
@@ -6466,12 +6470,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="195" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F195" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="202" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F202" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
translated and layout demo 52-54
</commit_message>
<xml_diff>
--- a/book/demos/Overview_demos.xlsx
+++ b/book/demos/Overview_demos.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suzan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ella\Documents\TU\Git\Showing-Physics\book\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8248FA62-BD24-47FC-BCE6-2174B17AD22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A76B470-80C5-4B03-875F-641CCAD4812A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1152" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="181">
   <si>
     <t>Demo name</t>
   </si>
@@ -566,6 +577,9 @@
   </si>
   <si>
     <t>Rich boiling phenomena</t>
+  </si>
+  <si>
+    <t>mis tekst</t>
   </si>
 </sst>
 </file>
@@ -697,9 +711,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -737,7 +751,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -843,7 +857,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -985,7 +999,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,9 +1009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2390,7 +2404,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>50</v>
       </c>
@@ -2407,7 +2421,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>51</v>
       </c>
@@ -2427,7 +2441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>52</v>
       </c>
@@ -2443,8 +2457,11 @@
       <c r="F67" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>53</v>
       </c>
@@ -2460,8 +2477,11 @@
       <c r="F68" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>54</v>
       </c>
@@ -2477,8 +2497,11 @@
       <c r="F69" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>55</v>
       </c>
@@ -2494,8 +2517,11 @@
       <c r="F70" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>56</v>
       </c>
@@ -2511,8 +2537,11 @@
       <c r="F71" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I71" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>57</v>
       </c>
@@ -2528,8 +2557,11 @@
       <c r="F72" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H72" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>58</v>
       </c>
@@ -2546,8 +2578,11 @@
         <v>73</v>
       </c>
       <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I73" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74">
         <v>59</v>
       </c>
@@ -2564,8 +2599,11 @@
         <v>72</v>
       </c>
       <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>60</v>
       </c>
@@ -2582,8 +2620,11 @@
         <v>71</v>
       </c>
       <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I75" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>61</v>
       </c>
@@ -2600,8 +2641,11 @@
         <v>70</v>
       </c>
       <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I76" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>62</v>
       </c>
@@ -2618,8 +2662,11 @@
         <v>119</v>
       </c>
       <c r="G77" s="6"/>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I77" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>63</v>
       </c>
@@ -2633,8 +2680,11 @@
         <v>79</v>
       </c>
       <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>64</v>
       </c>
@@ -2651,8 +2701,11 @@
         <v>78</v>
       </c>
       <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>65</v>
       </c>
@@ -2669,6 +2722,9 @@
         <v>77</v>
       </c>
       <c r="G80" s="2"/>
+      <c r="I80" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81">
@@ -2687,6 +2743,9 @@
         <v>76</v>
       </c>
       <c r="G81" s="2"/>
+      <c r="I81" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82">
@@ -2706,6 +2765,9 @@
       </c>
       <c r="H82" s="6" t="s">
         <v>173</v>
+      </c>
+      <c r="I82" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.3">

</xml_diff>